<commit_message>
Part way done with DP2 report
</commit_message>
<xml_diff>
--- a/dp_02/receiver/noise_budget.xlsx
+++ b/dp_02/receiver/noise_budget.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kavidey/Sync/Mudd/FA24/E157/dp_02/receiver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E79DF1-3311-5D41-B7AF-2F3D2B877D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4150B313-C50F-4B43-BEFD-BF2D0280BA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Stage</t>
   </si>
@@ -84,13 +85,184 @@
   </si>
   <si>
     <t>30 dB Attenuator</t>
+  </si>
+  <si>
+    <t>TX Noise</t>
+  </si>
+  <si>
+    <t>RX Noise</t>
+  </si>
+  <si>
+    <t>Stage 1</t>
+  </si>
+  <si>
+    <t>Stage 2</t>
+  </si>
+  <si>
+    <t>Stage 3</t>
+  </si>
+  <si>
+    <t>Stage 4</t>
+  </si>
+  <si>
+    <t>Stage 5</t>
+  </si>
+  <si>
+    <t>Stage 6</t>
+  </si>
+  <si>
+    <t>Wide BPF</t>
+  </si>
+  <si>
+    <t>Amplifier</t>
+  </si>
+  <si>
+    <t>Mixer</t>
+  </si>
+  <si>
+    <t>Narrow BPF</t>
+  </si>
+  <si>
+    <t>Attenuator</t>
+  </si>
+  <si>
+    <t>LPF</t>
+  </si>
+  <si>
+    <t>Stage 7</t>
+  </si>
+  <si>
+    <t>Stage 8</t>
+  </si>
+  <si>
+    <t>Stage 9</t>
+  </si>
+  <si>
+    <t>Transmit Antenna</t>
+  </si>
+  <si>
+    <t>Antenna Return Loss [dB]</t>
+  </si>
+  <si>
+    <t>Antenna Directionality [dBi]</t>
+  </si>
+  <si>
+    <t>Receive Antenna</t>
+  </si>
+  <si>
+    <t>Physical Parameters</t>
+  </si>
+  <si>
+    <t>Distance [m]</t>
+  </si>
+  <si>
+    <t>VBFZ-2340-S+ BPF</t>
+  </si>
+  <si>
+    <t>Insertion Loss [dB]</t>
+  </si>
+  <si>
+    <t>Band Start [MHz]</t>
+  </si>
+  <si>
+    <t>Band Stop [MHz]</t>
+  </si>
+  <si>
+    <t>ZX60-2531MA+ Amplifier</t>
+  </si>
+  <si>
+    <t>Gain @ 2200 MHz [dB]</t>
+  </si>
+  <si>
+    <t>Gain @ 300 MHz [dB]</t>
+  </si>
+  <si>
+    <t>IIP3 [dB]</t>
+  </si>
+  <si>
+    <t>OIP3 [dB]</t>
+  </si>
+  <si>
+    <t>ZX05-C24+ Mixer</t>
+  </si>
+  <si>
+    <t>Conversion Loss [dB]</t>
+  </si>
+  <si>
+    <t>Custom BPF</t>
+  </si>
+  <si>
+    <t>226 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>386 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>200 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>450 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>ZFL-1000LN Amplifier</t>
+  </si>
+  <si>
+    <t>Gain [dB]</t>
+  </si>
+  <si>
+    <t>ZX75LP-40-S+ LPF</t>
+  </si>
+  <si>
+    <t>75 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>100 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>150 MHz Attenuation [dB]</t>
+  </si>
+  <si>
+    <t>Physical Temperature [K]</t>
+  </si>
+  <si>
+    <t>NF [dB]</t>
+  </si>
+  <si>
+    <t>Stage Noise Contribution Theory [K]</t>
+  </si>
+  <si>
+    <t>Total Noise Temperature Theory [K]</t>
+  </si>
+  <si>
+    <t>Spectrum Analyzer Measurement DANL [dB]</t>
+  </si>
+  <si>
+    <t>Receiver Noise Measurement [dB]</t>
+  </si>
+  <si>
+    <t>Total Noise Temperature Theory [dB]</t>
+  </si>
+  <si>
+    <t>Boltzmann's Constant</t>
+  </si>
+  <si>
+    <t>Spectrum Analyzer</t>
+  </si>
+  <si>
+    <t>Noise Temperature [K]</t>
+  </si>
+  <si>
+    <t>Spectrum Analyzer RBW [Hz]</t>
+  </si>
+  <si>
+    <t>Receiver Noise Measurement [K]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -105,6 +277,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -132,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -140,6 +320,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,14 +535,729 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06FD6A6-1327-AC4F-B70D-750B4FADE777}">
+  <dimension ref="A1:S54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="7"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>290</v>
+      </c>
+      <c r="D3" s="4">
+        <f>(1/$S$23 - 1) *$R$8</f>
+        <v>110.31143673483658</v>
+      </c>
+      <c r="E3" s="4">
+        <f>($S$32-1)*$R$8</f>
+        <v>288.6260713409751</v>
+      </c>
+      <c r="F3" s="4">
+        <f>(1/$S$35 - 1) *$R$8</f>
+        <v>864.51079460514211</v>
+      </c>
+      <c r="G3" s="4">
+        <f>(1/POWER(10,-$R$38/10) - 1) *$R$8</f>
+        <v>738.95882877736904</v>
+      </c>
+      <c r="H3" s="4">
+        <f>(POWER(10,$R$32/10)-1)*$R$8</f>
+        <v>288.6260713409751</v>
+      </c>
+      <c r="I3" s="4">
+        <f>(1/POWER(10,-3/10) - 1) *$R$8</f>
+        <v>288.6260713409751</v>
+      </c>
+      <c r="J3" s="4">
+        <f>(POWER(10,$R$48/10)-1)*$R$8</f>
+        <v>275.45493392983315</v>
+      </c>
+      <c r="K3" s="4">
+        <f>(1/POWER(10,-$R$35/10) - 1) *$R$8</f>
+        <v>864.51079460514211</v>
+      </c>
+      <c r="L3" s="4">
+        <f>(1/POWER(10,-$R$51/10) - 1) *$R$8</f>
+        <v>75.08836942030851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="4">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <f>C3+B3</f>
+        <v>290</v>
+      </c>
+      <c r="D4" s="4">
+        <f>$S$23*(C4 + D3)</f>
+        <v>290</v>
+      </c>
+      <c r="E4" s="4">
+        <f>(D4+E3)*$S$28</f>
+        <v>2900000.0000000061</v>
+      </c>
+      <c r="F4" s="4">
+        <f>2*$S$35*(F3+E4)</f>
+        <v>1457328.440862532</v>
+      </c>
+      <c r="G4" s="4">
+        <f>$S$38*(F4 + G3)</f>
+        <v>410939.22719231312</v>
+      </c>
+      <c r="H4" s="4">
+        <f>(G4+H3)*$S$28</f>
+        <v>2061021501.6769304</v>
+      </c>
+      <c r="I4" s="4">
+        <f>POWER(10, -3/10)*(H4 + I3)</f>
+        <v>1032957809.5274895</v>
+      </c>
+      <c r="J4" s="4">
+        <f>(I4+J3)*$S$45</f>
+        <v>206102233990.78513</v>
+      </c>
+      <c r="K4" s="4">
+        <f>2*$S$35*(K3+J4)</f>
+        <v>103541081447.36374</v>
+      </c>
+      <c r="L4" s="4">
+        <f>$S$51*(K4 + L3)</f>
+        <v>82245604507.172302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6">
+        <f>10*LOG10(C4*C7*$R$9*1000)</f>
+        <v>-133.97518719422811</v>
+      </c>
+      <c r="D5" s="6">
+        <f>10*LOG10(D4*D7*$R$9*1000)</f>
+        <v>-133.97518719422811</v>
+      </c>
+      <c r="E5" s="6">
+        <f>10*LOG10(E4*E7*$R$9*1000)</f>
+        <v>-93.975187194228084</v>
+      </c>
+      <c r="F5" s="6">
+        <f>10*LOG10(F4*F7*$R$9*1000)</f>
+        <v>-86.963592767532219</v>
+      </c>
+      <c r="G5" s="6">
+        <f>10*LOG10(G4*G7*$R$9*1000)</f>
+        <v>-97.690178627371097</v>
+      </c>
+      <c r="H5" s="6">
+        <f>10*LOG10(H4*H7*$R$9*1000)</f>
+        <v>-60.687129400073005</v>
+      </c>
+      <c r="I5" s="6">
+        <f>10*LOG10(I4*I7*$R$9*1000)</f>
+        <v>-63.687128791885748</v>
+      </c>
+      <c r="J5" s="6">
+        <f>10*LOG10(J4*J7*$R$9*1000)</f>
+        <v>-40.687127633769308</v>
+      </c>
+      <c r="K5" s="6">
+        <f>10*LOG10(K4*K7*$R$9*1000)</f>
+        <v>-48.448040206109326</v>
+      </c>
+      <c r="L5" s="6">
+        <f>10*LOG10(L4*L7*$R$9*1000)</f>
+        <v>-44.676827655763176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="H7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="I7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="J7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="K7" s="4">
+        <v>10000</v>
+      </c>
+      <c r="L7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="6">
+        <f>10*LOG10(C7*$R$12*$R$9*1000)</f>
+        <v>-70.001781511246193</v>
+      </c>
+      <c r="D8" s="6">
+        <f>10*LOG10(D7*$R$12*$R$9*1000)</f>
+        <v>-70.001781511246193</v>
+      </c>
+      <c r="E8" s="6">
+        <f>10*LOG10(E7*$R$12*$R$9*1000)</f>
+        <v>-70.001781511246193</v>
+      </c>
+      <c r="F8" s="6">
+        <f>10*LOG10(F7*$R$12*$R$9*1000)</f>
+        <v>-60.001781511246193</v>
+      </c>
+      <c r="G8" s="6">
+        <f>10*LOG10(G7*$R$12*$R$9*1000)</f>
+        <v>-65.230568964049567</v>
+      </c>
+      <c r="H8" s="6">
+        <f>10*LOG10(H7*$R$12*$R$9*1000)</f>
+        <v>-65.230568964049567</v>
+      </c>
+      <c r="I8" s="6">
+        <f>10*LOG10(I7*$R$12*$R$9*1000)</f>
+        <v>-65.230568964049567</v>
+      </c>
+      <c r="J8" s="6">
+        <f>10*LOG10(J7*$R$12*$R$9*1000)</f>
+        <v>-65.230568964049567</v>
+      </c>
+      <c r="K8" s="6">
+        <f>10*LOG10(K7*$R$12*$R$9*1000)</f>
+        <v>-70.001781511246193</v>
+      </c>
+      <c r="L8" s="6">
+        <f>10*LOG10(L7*$R$12*$R$9*1000)</f>
+        <v>-65.230568964049567</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>-71.099999999999994</v>
+      </c>
+      <c r="D9">
+        <v>-69.5</v>
+      </c>
+      <c r="E9">
+        <v>-69.8</v>
+      </c>
+      <c r="F9">
+        <v>-61.9</v>
+      </c>
+      <c r="G9">
+        <v>-75.099999999999994</v>
+      </c>
+      <c r="H9">
+        <v>-68.2</v>
+      </c>
+      <c r="I9">
+        <v>-70.3</v>
+      </c>
+      <c r="J9">
+        <v>-51.5</v>
+      </c>
+      <c r="K9">
+        <v>-74.8</v>
+      </c>
+      <c r="L9">
+        <v>-75.3</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9">
+        <f>1.380649E-23</f>
+        <v>1.3806490000000001E-23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="4">
+        <f>POWER(10,C9/10) / (1000 * $R$9*C7)</f>
+        <v>562233497.89026177</v>
+      </c>
+      <c r="D10" s="4">
+        <f>POWER(10,D9/10) / (1000 * $R$9*D7)</f>
+        <v>812674658.29617965</v>
+      </c>
+      <c r="E10" s="4">
+        <f>POWER(10,E9/10) / (1000 * $R$9*E7)</f>
+        <v>758432120.00363505</v>
+      </c>
+      <c r="F10" s="4">
+        <f>POWER(10,F9/10) / (1000 * $R$9*F7)</f>
+        <v>467645454.44544977</v>
+      </c>
+      <c r="G10" s="4">
+        <f>POWER(10,G9/10) / (1000 * $R$9*G7)</f>
+        <v>74609729.011829004</v>
+      </c>
+      <c r="H10" s="4">
+        <f>POWER(10,H9/10) / (1000 * $R$9*H7)</f>
+        <v>365422649.88813341</v>
+      </c>
+      <c r="I10" s="4">
+        <f>POWER(10,I9/10) / (1000 * $R$9*I7)</f>
+        <v>225317779.48800182</v>
+      </c>
+      <c r="J10" s="4">
+        <f>POWER(10,J9/10) / (1000 * $R$9*J7)</f>
+        <v>17092101477.496843</v>
+      </c>
+      <c r="K10" s="4">
+        <f>POWER(10,K9/10) / (1000 * $R$9*K7)</f>
+        <v>239837294.98416415</v>
+      </c>
+      <c r="L10" s="4">
+        <f>POWER(10,L9/10) / (1000 * $R$9*L7)</f>
+        <v>71251738.051365405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="4">
+        <v>724000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R15" s="1">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="Q16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q18" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="1">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="20" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q22" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R23">
+        <v>1.4</v>
+      </c>
+      <c r="S23">
+        <f>POWER(10,-R23/10)</f>
+        <v>0.72443596007499012</v>
+      </c>
+    </row>
+    <row r="24" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="25" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R25">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="27" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q27" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R28">
+        <v>37</v>
+      </c>
+      <c r="S28">
+        <f>POWER(10,R28/10)</f>
+        <v>5011.8723362727324</v>
+      </c>
+    </row>
+    <row r="29" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R29">
+        <v>35</v>
+      </c>
+      <c r="S29">
+        <f>POWER(10,R29/10)</f>
+        <v>3162.2776601683804</v>
+      </c>
+    </row>
+    <row r="30" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R30" s="2">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="31" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R31" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R32" s="2">
+        <v>3</v>
+      </c>
+      <c r="S32">
+        <f>POWER(10,R32/10)</f>
+        <v>1.9952623149688797</v>
+      </c>
+    </row>
+    <row r="34" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q34" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R35">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <f>POWER(10,-R35/10)</f>
+        <v>0.25118864315095801</v>
+      </c>
+    </row>
+    <row r="37" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q37" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R38">
+        <v>5.5</v>
+      </c>
+      <c r="S38">
+        <f>POWER(10,-R38/10)</f>
+        <v>0.28183829312644532</v>
+      </c>
+    </row>
+    <row r="39" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R41">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q44" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q45" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R45">
+        <v>23</v>
+      </c>
+      <c r="S45">
+        <f>POWER(10,R45/10)</f>
+        <v>199.52623149688802</v>
+      </c>
+    </row>
+    <row r="46" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R46" s="2">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="47" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R47" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q48" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R48" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="S48">
+        <f>POWER(10,R48/10)</f>
+        <v>1.9498445997580454</v>
+      </c>
+    </row>
+    <row r="50" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q50" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <f>POWER(10,-R51/10)</f>
+        <v>0.79432823472428149</v>
+      </c>
+    </row>
+    <row r="52" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R52">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="17:19" x14ac:dyDescent="0.15">
+      <c r="Q54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R54">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>